<commit_message>
Lagt till i planering
</commit_message>
<xml_diff>
--- a/Programmering/Dokument/Planering inför SGA.xlsx
+++ b/Programmering/Dokument/Planering inför SGA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Hjälpvideos</t>
   </si>
@@ -67,13 +67,16 @@
   </si>
   <si>
     <t>Buggfixar etc</t>
+  </si>
+  <si>
+    <t>Rörliga objekt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +97,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -129,7 +139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -140,6 +150,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -162,7 +173,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="21" formatCode="dd/mmm"/>
     </dxf>
     <dxf>
       <font>
@@ -180,6 +190,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="21" formatCode="dd/mmm"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -193,10 +204,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:F12" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:F12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:F13" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:F13"/>
   <tableColumns count="6">
-    <tableColumn id="1" name=" " dataDxfId="1"/>
+    <tableColumn id="1" name=" " dataDxfId="0"/>
     <tableColumn id="2" name="05-maj"/>
     <tableColumn id="3" name="12-maj"/>
     <tableColumn id="4" name="19-maj"/>
@@ -492,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -538,63 +549,69 @@
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="6" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="6" t="s">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="6" t="s">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="6" t="s">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="6" t="s">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="6" t="s">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="6" t="s">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="7" t="s">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>